<commit_message>
feat: add event categories to admin panel and refine admin UI
</commit_message>
<xml_diff>
--- a/Olkkari Wines.xlsx
+++ b/Olkkari Wines.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunom\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunom\Documents\ravinteli-olkkari\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2826553-203A-4B80-8696-60ABB86FC14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10BD6A0-1EE5-4815-B365-B5B689B6C546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="2835" windowWidth="21600" windowHeight="11295" xr2:uid="{82D3A307-4FE3-43E4-B060-BCDAE2976B50}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -601,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0405DAB4-7152-44BA-B4F3-517816F9B896}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
       <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
@@ -610,7 +611,7 @@
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -650,7 +651,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -670,7 +671,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -690,7 +691,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -710,7 +711,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -730,7 +731,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -750,7 +751,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -770,7 +771,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -790,7 +791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -810,7 +811,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -830,7 +831,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -850,7 +851,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>27</v>
       </c>
@@ -870,7 +871,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -890,7 +891,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -910,7 +911,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
@@ -930,7 +931,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -950,7 +951,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
@@ -970,7 +971,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>27</v>
       </c>
@@ -990,7 +991,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>27</v>
       </c>
@@ -1010,7 +1011,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1030,7 +1031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>27</v>
       </c>
@@ -1050,7 +1051,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1070,7 +1071,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>48</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>

</xml_diff>